<commit_message>
added dives to dive log
</commit_message>
<xml_diff>
--- a/documents/DiveLog.xlsx
+++ b/documents/DiveLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d05eacb21039f7c7/Active_Projects/Washington_Coast_Benthic_Surveys/ROV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d05eacb21039f7c7/Active_Projects/Washington_Coast_Benthic_Surveys/GitHub/Seattle_Aquarium_ROV/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="468" documentId="8_{91C2599B-E2FB-4CCD-A0A1-1D7B97CCE226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72EF241A-D010-4D95-AA83-156FC5F0E98C}"/>
+  <xr:revisionPtr revIDLastSave="475" documentId="8_{91C2599B-E2FB-4CCD-A0A1-1D7B97CCE226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9999BD7D-77BA-4A12-9D41-B90BAB168436}"/>
   <bookViews>
-    <workbookView xWindow="21490" yWindow="6410" windowWidth="38620" windowHeight="21220" xr2:uid="{2838E10B-E91C-44A4-ACAD-D860EA172BA9}"/>
+    <workbookView xWindow="21490" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{2838E10B-E91C-44A4-ACAD-D860EA172BA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="103">
   <si>
     <t>BlueROV2 Operations Log</t>
   </si>
@@ -262,9 +262,6 @@
     <t xml:space="preserve">operator </t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>312 730 4842</t>
   </si>
   <si>
@@ -308,13 +305,52 @@
   </si>
   <si>
     <t>425 750 6645</t>
+  </si>
+  <si>
+    <t>Pier 59 West OTS</t>
+  </si>
+  <si>
+    <t>test light shroud, Ping sonar, and trim/handling with additional hardware; first dive with forward-facing GoPro</t>
+  </si>
+  <si>
+    <t>Ping worked well; light shroud worked well; ROV negatively bouyant and lists forward slightly; NOTE to adjust ballast and ideally retest trim in holding tank</t>
+  </si>
+  <si>
+    <t>Pier 62</t>
+  </si>
+  <si>
+    <t>shore</t>
+  </si>
+  <si>
+    <t>Test engagement with CEaL; perform structured tests of light power across varying ROV altitudes</t>
+  </si>
+  <si>
+    <t>Mike Smith</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Hollander</t>
+  </si>
+  <si>
+    <t>Joel Hollander</t>
+  </si>
+  <si>
+    <t>Seattle Aquarium LS</t>
+  </si>
+  <si>
+    <t>206 714 8968</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +394,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -509,7 +558,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -572,6 +621,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -892,36 +953,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E01455-1EBD-4852-BC5D-52B881F45A58}">
-  <dimension ref="A1:X115"/>
+  <dimension ref="A1:Y112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="3"/>
-    <col min="2" max="2" width="13.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="3" customWidth="1"/>
-    <col min="7" max="9" width="18.5703125" style="3" customWidth="1"/>
-    <col min="10" max="12" width="11.85546875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="3"/>
+    <col min="2" max="2" width="13.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" style="3" customWidth="1"/>
+    <col min="7" max="9" width="18.54296875" style="3" customWidth="1"/>
+    <col min="10" max="12" width="11.81640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="16.81640625" style="3" customWidth="1"/>
     <col min="14" max="16" width="17" style="3" customWidth="1"/>
-    <col min="17" max="17" width="18.7109375" style="3" customWidth="1"/>
-    <col min="18" max="18" width="23.85546875" style="3" customWidth="1"/>
-    <col min="19" max="19" width="18.85546875" style="3" customWidth="1"/>
-    <col min="20" max="20" width="52.85546875" style="3" customWidth="1"/>
+    <col min="17" max="17" width="18.7265625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="23.81640625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="18.81640625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="52.81640625" style="3" customWidth="1"/>
     <col min="21" max="21" width="25" style="3" customWidth="1"/>
-    <col min="22" max="22" width="16.140625" style="3" customWidth="1"/>
-    <col min="23" max="23" width="17.5703125" style="3" customWidth="1"/>
+    <col min="22" max="22" width="16.1796875" style="3" customWidth="1"/>
+    <col min="23" max="23" width="17.54296875" style="3" customWidth="1"/>
     <col min="24" max="24" width="15" style="3" customWidth="1"/>
-    <col min="25" max="16384" width="8.7109375" style="3"/>
+    <col min="25" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -947,7 +1008,7 @@
       </c>
       <c r="T1" s="19"/>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="15.75">
+    <row r="2" spans="1:25" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1009,7 +1070,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -1071,7 +1132,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -1133,7 +1194,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -1195,7 +1256,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="15">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -1257,59 +1318,125 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9" t="s">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A7" s="22">
+        <v>5</v>
+      </c>
+      <c r="B7" s="23">
+        <v>44679</v>
+      </c>
+      <c r="C7" s="24">
+        <v>0.625</v>
+      </c>
+      <c r="D7" s="22">
+        <v>31</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="R7" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="S7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="T7" s="9" t="s">
+      <c r="T7" s="22" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" ht="15">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9" t="s">
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="25"/>
+      <c r="X7" s="25"/>
+      <c r="Y7" s="25"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A8" s="22">
+        <v>6</v>
+      </c>
+      <c r="B8" s="23">
+        <v>44684</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T8" s="9" t="s">
+      <c r="T8" s="22" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" ht="15">
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="25"/>
+      <c r="X8" s="25"/>
+      <c r="Y8" s="25"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -1335,7 +1462,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1361,7 +1488,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -1387,7 +1514,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="15">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -1413,7 +1540,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="15">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -1439,7 +1566,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="15">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -1465,7 +1592,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="15">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -1491,7 +1618,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="15">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -1517,7 +1644,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="15">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -1543,7 +1670,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="15">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -1569,7 +1696,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="15">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -1595,7 +1722,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="15">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -1621,7 +1748,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="15">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -1643,7 +1770,7 @@
       <c r="S21" s="9"/>
       <c r="T21" s="9"/>
     </row>
-    <row r="22" spans="1:24" ht="15">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -1667,7 +1794,7 @@
       </c>
       <c r="T22" s="20"/>
     </row>
-    <row r="23" spans="1:24" ht="15">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1693,7 +1820,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="15">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -1717,10 +1844,10 @@
       </c>
       <c r="T24" s="12">
         <f>SUM(D:D)</f>
-        <v>207</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" ht="15">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -1744,10 +1871,10 @@
       </c>
       <c r="T25" s="9">
         <f>T24/COUNT(A:A)</f>
-        <v>51.75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" ht="15">
+        <v>39.666666666666664</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -1771,10 +1898,10 @@
       </c>
       <c r="T26" s="9">
         <f>COUNT(A:A)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" ht="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1800,7 +1927,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="15">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1820,7 +1947,7 @@
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
     </row>
-    <row r="29" spans="1:24" ht="15">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1848,7 +1975,7 @@
       <c r="W29" s="21"/>
       <c r="X29" s="21"/>
     </row>
-    <row r="30" spans="1:24" ht="15">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1886,7 +2013,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="15">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1918,13 +2045,13 @@
         <v>74</v>
       </c>
       <c r="W31" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="X31" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="X31" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="15">
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1947,22 +2074,22 @@
         <v>27</v>
       </c>
       <c r="T32" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="U32" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="U32" s="3" t="s">
+      <c r="V32" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="V32" s="3" t="s">
+      <c r="W32" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="X32" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="W32" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="X32" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" ht="15">
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1982,25 +2109,25 @@
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
       <c r="S33" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="T33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="T33" s="3" t="s">
+      <c r="U33" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="V33" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="U33" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="V33" s="3" t="s">
+      <c r="W33" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="X33" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="W33" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="X33" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" ht="15">
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2020,25 +2147,25 @@
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
       <c r="S34" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="T34" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="T34" s="3" t="s">
+      <c r="U34" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="V34" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="W34" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="X34" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="U34" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="V34" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="W34" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="X34" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" ht="15">
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2061,22 +2188,22 @@
         <v>36</v>
       </c>
       <c r="T35" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U35" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="U35" s="3" t="s">
+      <c r="V35" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="W35" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="X35" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="V35" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="W35" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="X35" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" ht="15">
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2095,8 +2222,26 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
-    </row>
-    <row r="37" spans="1:24" ht="15">
+      <c r="S36" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="T36" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="U36" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="V36" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="W36" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="X36" s="25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2116,7 +2261,7 @@
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
     </row>
-    <row r="38" spans="1:24" ht="15">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2136,7 +2281,7 @@
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
     </row>
-    <row r="39" spans="1:24" ht="15">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2156,7 +2301,7 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
     </row>
-    <row r="40" spans="1:24" ht="15">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2176,7 +2321,7 @@
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
     </row>
-    <row r="41" spans="1:24" ht="15">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2196,7 +2341,7 @@
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
     </row>
-    <row r="42" spans="1:24" ht="15">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2216,7 +2361,7 @@
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
     </row>
-    <row r="43" spans="1:24" ht="15">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2236,7 +2381,7 @@
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
     </row>
-    <row r="44" spans="1:24" ht="15">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2256,7 +2401,7 @@
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
     </row>
-    <row r="45" spans="1:24" ht="15">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2276,7 +2421,7 @@
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
     </row>
-    <row r="46" spans="1:24" ht="15">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2296,7 +2441,7 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
-    <row r="47" spans="1:24" ht="15">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2316,7 +2461,7 @@
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
     </row>
-    <row r="48" spans="1:24" ht="15">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2336,7 +2481,7 @@
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
     </row>
-    <row r="49" spans="1:18" ht="15">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2356,7 +2501,7 @@
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
     </row>
-    <row r="50" spans="1:18" ht="15">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2376,7 +2521,7 @@
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
     </row>
-    <row r="51" spans="1:18" ht="15">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2396,7 +2541,7 @@
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
     </row>
-    <row r="52" spans="1:18" ht="15">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2416,7 +2561,7 @@
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
     </row>
-    <row r="53" spans="1:18" ht="15">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2436,7 +2581,7 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="1:18" ht="15">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2456,7 +2601,7 @@
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
     </row>
-    <row r="55" spans="1:18" ht="15">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2476,7 +2621,7 @@
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
     </row>
-    <row r="56" spans="1:18" ht="15">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2496,7 +2641,7 @@
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
     </row>
-    <row r="57" spans="1:18" ht="15">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2516,7 +2661,7 @@
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
     </row>
-    <row r="58" spans="1:18" ht="15">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2536,7 +2681,7 @@
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
     </row>
-    <row r="59" spans="1:18" ht="15">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2556,7 +2701,7 @@
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
     </row>
-    <row r="60" spans="1:18" ht="15">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2576,7 +2721,7 @@
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
     </row>
-    <row r="61" spans="1:18" ht="15">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2596,7 +2741,7 @@
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
     </row>
-    <row r="62" spans="1:18" ht="15">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2616,7 +2761,7 @@
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
     </row>
-    <row r="63" spans="1:18" ht="15">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2636,7 +2781,7 @@
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
     </row>
-    <row r="64" spans="1:18" ht="15">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2656,7 +2801,7 @@
       <c r="Q64" s="2"/>
       <c r="R64" s="2"/>
     </row>
-    <row r="65" spans="1:18" ht="15">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2676,7 +2821,7 @@
       <c r="Q65" s="2"/>
       <c r="R65" s="2"/>
     </row>
-    <row r="66" spans="1:18" ht="15">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2696,7 +2841,7 @@
       <c r="Q66" s="2"/>
       <c r="R66" s="2"/>
     </row>
-    <row r="67" spans="1:18" ht="15">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2716,7 +2861,7 @@
       <c r="Q67" s="2"/>
       <c r="R67" s="2"/>
     </row>
-    <row r="68" spans="1:18" ht="15">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2736,7 +2881,7 @@
       <c r="Q68" s="2"/>
       <c r="R68" s="2"/>
     </row>
-    <row r="69" spans="1:18" ht="15">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2756,7 +2901,7 @@
       <c r="Q69" s="2"/>
       <c r="R69" s="2"/>
     </row>
-    <row r="70" spans="1:18" ht="15">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2776,7 +2921,7 @@
       <c r="Q70" s="2"/>
       <c r="R70" s="2"/>
     </row>
-    <row r="71" spans="1:18" ht="15">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2796,7 +2941,7 @@
       <c r="Q71" s="2"/>
       <c r="R71" s="2"/>
     </row>
-    <row r="72" spans="1:18" ht="15">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2816,7 +2961,7 @@
       <c r="Q72" s="2"/>
       <c r="R72" s="2"/>
     </row>
-    <row r="73" spans="1:18" ht="15">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2836,7 +2981,7 @@
       <c r="Q73" s="2"/>
       <c r="R73" s="2"/>
     </row>
-    <row r="74" spans="1:18" ht="15">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2856,7 +3001,7 @@
       <c r="Q74" s="2"/>
       <c r="R74" s="2"/>
     </row>
-    <row r="75" spans="1:18" ht="15">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2876,7 +3021,7 @@
       <c r="Q75" s="2"/>
       <c r="R75" s="2"/>
     </row>
-    <row r="76" spans="1:18" ht="15">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2896,7 +3041,7 @@
       <c r="Q76" s="2"/>
       <c r="R76" s="2"/>
     </row>
-    <row r="77" spans="1:18" ht="15">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2916,7 +3061,7 @@
       <c r="Q77" s="2"/>
       <c r="R77" s="2"/>
     </row>
-    <row r="78" spans="1:18" ht="15">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2936,7 +3081,7 @@
       <c r="Q78" s="2"/>
       <c r="R78" s="2"/>
     </row>
-    <row r="79" spans="1:18" ht="15">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2956,7 +3101,7 @@
       <c r="Q79" s="2"/>
       <c r="R79" s="2"/>
     </row>
-    <row r="80" spans="1:18" ht="15">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2976,7 +3121,7 @@
       <c r="Q80" s="2"/>
       <c r="R80" s="2"/>
     </row>
-    <row r="81" spans="1:18" ht="15">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2996,7 +3141,7 @@
       <c r="Q81" s="2"/>
       <c r="R81" s="2"/>
     </row>
-    <row r="82" spans="1:18" ht="15">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -3016,7 +3161,7 @@
       <c r="Q82" s="2"/>
       <c r="R82" s="2"/>
     </row>
-    <row r="83" spans="1:18" ht="15">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -3036,7 +3181,7 @@
       <c r="Q83" s="2"/>
       <c r="R83" s="2"/>
     </row>
-    <row r="84" spans="1:18" ht="15">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -3056,7 +3201,7 @@
       <c r="Q84" s="2"/>
       <c r="R84" s="2"/>
     </row>
-    <row r="85" spans="1:18" ht="15">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -3076,7 +3221,7 @@
       <c r="Q85" s="2"/>
       <c r="R85" s="2"/>
     </row>
-    <row r="86" spans="1:18" ht="15">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -3096,7 +3241,7 @@
       <c r="Q86" s="2"/>
       <c r="R86" s="2"/>
     </row>
-    <row r="87" spans="1:18" ht="15">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -3116,7 +3261,7 @@
       <c r="Q87" s="2"/>
       <c r="R87" s="2"/>
     </row>
-    <row r="88" spans="1:18" ht="15">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -3136,7 +3281,7 @@
       <c r="Q88" s="2"/>
       <c r="R88" s="2"/>
     </row>
-    <row r="89" spans="1:18" ht="15">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -3156,7 +3301,7 @@
       <c r="Q89" s="2"/>
       <c r="R89" s="2"/>
     </row>
-    <row r="90" spans="1:18" ht="15">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -3176,7 +3321,7 @@
       <c r="Q90" s="2"/>
       <c r="R90" s="2"/>
     </row>
-    <row r="91" spans="1:18" ht="15">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -3196,7 +3341,7 @@
       <c r="Q91" s="2"/>
       <c r="R91" s="2"/>
     </row>
-    <row r="92" spans="1:18" ht="15">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -3216,7 +3361,7 @@
       <c r="Q92" s="2"/>
       <c r="R92" s="2"/>
     </row>
-    <row r="93" spans="1:18" ht="15">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -3236,7 +3381,7 @@
       <c r="Q93" s="2"/>
       <c r="R93" s="2"/>
     </row>
-    <row r="94" spans="1:18" ht="15">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -3256,7 +3401,7 @@
       <c r="Q94" s="2"/>
       <c r="R94" s="2"/>
     </row>
-    <row r="95" spans="1:18" ht="15">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -3276,7 +3421,7 @@
       <c r="Q95" s="2"/>
       <c r="R95" s="2"/>
     </row>
-    <row r="96" spans="1:18" ht="15">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -3296,7 +3441,7 @@
       <c r="Q96" s="2"/>
       <c r="R96" s="2"/>
     </row>
-    <row r="97" spans="1:18" ht="15">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -3316,54 +3461,51 @@
       <c r="Q97" s="2"/>
       <c r="R97" s="2"/>
     </row>
-    <row r="98" spans="1:18" ht="15">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
     </row>
-    <row r="99" spans="1:18" ht="15">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
     </row>
-    <row r="100" spans="1:18" ht="15">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
     </row>
-    <row r="101" spans="1:18" ht="15">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
     </row>
-    <row r="102" spans="1:18" ht="15">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A102" s="2"/>
     </row>
-    <row r="103" spans="1:18" ht="15">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A103" s="2"/>
     </row>
-    <row r="104" spans="1:18" ht="15">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A104" s="2"/>
     </row>
-    <row r="105" spans="1:18" ht="15">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A105" s="2"/>
     </row>
-    <row r="106" spans="1:18" ht="15">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A106" s="2"/>
     </row>
-    <row r="107" spans="1:18" ht="15">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A107" s="2"/>
     </row>
-    <row r="108" spans="1:18" ht="15">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A108" s="2"/>
     </row>
-    <row r="109" spans="1:18" ht="15">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A109" s="2"/>
     </row>
-    <row r="110" spans="1:18" ht="15">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A110" s="2"/>
     </row>
-    <row r="111" spans="1:18" ht="15">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A111" s="2"/>
     </row>
-    <row r="112" spans="1:18" ht="15">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A112" s="2"/>
     </row>
-    <row r="113" ht="15"/>
-    <row r="114" ht="15"/>
-    <row r="115" ht="15"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:R1"/>
@@ -3377,6 +3519,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EB27F40EE1C55948AD7A8659B1C90754" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="502be3947e2cee2dcf68fa734ba74869">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef2479e3-ab94-4f56-9056-63fe784fb201" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b91b3180a99694d1a5a2659f6046e79" ns2:_="">
     <xsd:import namespace="ef2479e3-ab94-4f56-9056-63fe784fb201"/>
@@ -3566,29 +3723,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09F81F5B-0897-48FE-BD96-1B6E9597E582}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C81E9D3A-E160-43A0-8244-0564D59CB1A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74A583F9-58C6-4F7C-96D8-C86C94C0D0B3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74A583F9-58C6-4F7C-96D8-C86C94C0D0B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C81E9D3A-E160-43A0-8244-0564D59CB1A6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09F81F5B-0897-48FE-BD96-1B6E9597E582}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ef2479e3-ab94-4f56-9056-63fe784fb201"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>